<commit_message>
feat:Função do Botão Baixar e Selecionar
</commit_message>
<xml_diff>
--- a/app/planilhas/PComp-ceo-d.xlsx
+++ b/app/planilhas/PComp-ceo-d.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\William\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D_Muniz\Desktop\Teethgram\teethGram\app\planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FCF038-3D32-42B8-8C71-FCBDC471EFDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0079C078-8BF8-439C-B6D9-8FE6B8CAC1E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{AFFBEBE6-A6BC-498C-A820-BBF450B005CB}"/>
   </bookViews>
@@ -31,15 +31,12 @@
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>TOTAL Participantes</t>
   </si>
@@ -54,6 +51,9 @@
   </si>
   <si>
     <t>SOMA</t>
+  </si>
+  <si>
+    <t>Código</t>
   </si>
 </sst>
 </file>
@@ -494,7 +494,7 @@
   <dimension ref="A1:BA6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,6 +503,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="B1" s="3">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
docs: substitui planilhas antigas pela nova versão
</commit_message>
<xml_diff>
--- a/app/planilhas/PComp-ceo-d.xlsx
+++ b/app/planilhas/PComp-ceo-d.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\William\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D_Muniz\Desktop\Teethgram\teethGram\app\planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FCF038-3D32-42B8-8C71-FCBDC471EFDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0079C078-8BF8-439C-B6D9-8FE6B8CAC1E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{AFFBEBE6-A6BC-498C-A820-BBF450B005CB}"/>
   </bookViews>
@@ -31,15 +31,12 @@
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>TOTAL Participantes</t>
   </si>
@@ -54,6 +51,9 @@
   </si>
   <si>
     <t>SOMA</t>
+  </si>
+  <si>
+    <t>Código</t>
   </si>
 </sst>
 </file>
@@ -494,7 +494,7 @@
   <dimension ref="A1:BA6"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,6 +503,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>5</v>
+      </c>
       <c r="B1" s="3">
         <v>55</v>
       </c>

</xml_diff>